<commit_message>
adding copy of simple XY based figure building
</commit_message>
<xml_diff>
--- a/simple_X_Y/Deep Dive kinome Peptide parameters 022019.xlsx
+++ b/simple_X_Y/Deep Dive kinome Peptide parameters 022019.xlsx
@@ -146,7 +146,7 @@
     <t xml:space="preserve">y=1.01x-0.162</t>
   </si>
   <si>
-    <t xml:space="preserve">y=0.926x+0.106</t>
+    <t xml:space="preserve">y=0.037x+0.004</t>
   </si>
   <si>
     <t xml:space="preserve">LCGSPCPAVWPDVIK</t>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">y=1.10x-1.28</t>
   </si>
   <si>
-    <t xml:space="preserve">y=0.958x-0.316</t>
+    <t xml:space="preserve">y=0.038x-0.013</t>
   </si>
   <si>
     <t xml:space="preserve">CDK13 </t>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">y=1.106x-0.656</t>
   </si>
   <si>
-    <t xml:space="preserve">y=0.909x+0.161</t>
+    <t xml:space="preserve">y=0.036x+0.006</t>
   </si>
   <si>
     <t xml:space="preserve">VENNLIVDK</t>
@@ -179,7 +179,7 @@
     <t xml:space="preserve">y=1.03x-0.210</t>
   </si>
   <si>
-    <t xml:space="preserve">y=0.874x+0.150</t>
+    <t xml:space="preserve">y=0.035x+0.006</t>
   </si>
   <si>
     <t xml:space="preserve">PKMYT1</t>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">y=1.09x-0.158</t>
   </si>
   <si>
-    <t xml:space="preserve">y=0.934x+0.012</t>
+    <t xml:space="preserve">y=0.037x+0.000</t>
   </si>
   <si>
     <t xml:space="preserve">GSFPSFEPR</t>
@@ -203,7 +203,7 @@
     <t xml:space="preserve">y=1.01x-0.145</t>
   </si>
   <si>
-    <t xml:space="preserve">y=1.03x-0.090</t>
+    <t xml:space="preserve">y=0.041x-0.004</t>
   </si>
   <si>
     <t xml:space="preserve">SLPPPPPAK</t>
@@ -212,7 +212,7 @@
     <t xml:space="preserve">y=1.13x-0.408</t>
   </si>
   <si>
-    <t xml:space="preserve">y=0.859x-0.198</t>
+    <t xml:space="preserve">y=0.034x-0.008</t>
   </si>
   <si>
     <t xml:space="preserve">TLK2</t>
@@ -227,7 +227,7 @@
     <t xml:space="preserve">y=1.36x-0.048</t>
   </si>
   <si>
-    <t xml:space="preserve">y=0.739x-0.167</t>
+    <t xml:space="preserve">y=0.030x-0.007</t>
   </si>
   <si>
     <t xml:space="preserve">ISALENSK</t>
@@ -236,7 +236,7 @@
     <t xml:space="preserve">y=1.05x-0.298</t>
   </si>
   <si>
-    <t xml:space="preserve">y=1.10x-0.254</t>
+    <t xml:space="preserve">y=0.044x-0.010</t>
   </si>
   <si>
     <r>
@@ -519,7 +519,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>